<commit_message>
working date range report mail batch
</commit_message>
<xml_diff>
--- a/EEMReportFinal/EEMReport/EEMReport/Telus Dashboard.xlsx
+++ b/EEMReportFinal/EEMReport/EEMReport/Telus Dashboard.xlsx
@@ -28639,7 +28639,7 @@
         <v>144</v>
       </c>
       <c r="B2" t="n" s="103">
-        <v>43230.02899305556</v>
+        <v>43229.54578703704</v>
       </c>
       <c r="C2" t="n">
         <v>20.0</v>
@@ -28755,7 +28755,7 @@
         <v>149</v>
       </c>
       <c r="B3" t="n" s="104">
-        <v>43230.02900462963</v>
+        <v>43229.548368055555</v>
       </c>
       <c r="C3" t="n">
         <v>30.0</v>
@@ -28871,7 +28871,7 @@
         <v>151</v>
       </c>
       <c r="B4" t="n" s="105">
-        <v>43230.02900462963</v>
+        <v>43229.54976851852</v>
       </c>
       <c r="C4" t="n">
         <v>40.0</v>
@@ -28987,7 +28987,7 @@
         <v>152</v>
       </c>
       <c r="B5" t="n" s="106">
-        <v>43230.02900462963</v>
+        <v>43229.55069444444</v>
       </c>
       <c r="C5" t="n">
         <v>70.0</v>
@@ -29103,7 +29103,7 @@
         <v>153</v>
       </c>
       <c r="B6" t="n" s="107">
-        <v>43230.02900462963</v>
+        <v>43229.55196759259</v>
       </c>
       <c r="C6" t="n">
         <v>20.0</v>
@@ -29408,7 +29408,7 @@
         <v>144</v>
       </c>
       <c r="B2" t="n" s="98">
-        <v>43242.006261574075</v>
+        <v>43236.65914351852</v>
       </c>
       <c r="C2" t="n">
         <v>20.0</v>
@@ -29530,7 +29530,7 @@
         <v>144</v>
       </c>
       <c r="B3" t="n" s="99">
-        <v>43242.006261574075</v>
+        <v>43236.66354166667</v>
       </c>
       <c r="C3" t="n">
         <v>10.0</v>
@@ -29652,7 +29652,7 @@
         <v>144</v>
       </c>
       <c r="B4" t="n" s="100">
-        <v>43242.006261574075</v>
+        <v>43236.66354166667</v>
       </c>
       <c r="C4" t="n">
         <v>10.0</v>
@@ -29774,7 +29774,7 @@
         <v>144</v>
       </c>
       <c r="B5" t="n" s="101">
-        <v>43242.006273148145</v>
+        <v>43236.66354166667</v>
       </c>
       <c r="C5" t="n">
         <v>10.0</v>
@@ -29896,7 +29896,7 @@
         <v>149</v>
       </c>
       <c r="B6" t="n" s="102">
-        <v>43242.006273148145</v>
+        <v>43236.66354166667</v>
       </c>
       <c r="C6" t="n">
         <v>101.0</v>

</xml_diff>